<commit_message>
Reporte de docentes- Agregado
</commit_message>
<xml_diff>
--- a/public/Plantillas/Reporte-Proyectos.xlsx
+++ b/public/Plantillas/Reporte-Proyectos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ESPE_2023\sistema_vinculacion\sistema_vinculacion\public\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\TesisVersionBeta\public\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B84519-1BB6-45D8-9130-D1031F1B7BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CD7DE0-E4C7-45D4-9601-4A1C6BB44511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E868ECBF-1759-4E94-BEB5-846D8DEB5231}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,27 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>N|</t>
   </si>
   <si>
     <t>Fecha Inicio</t>
-  </si>
-  <si>
-    <t>Reporte Proyectos Vinculacion a la sociedad</t>
-  </si>
-  <si>
-    <t>Nombre del Proyecto</t>
-  </si>
-  <si>
-    <t>Director</t>
-  </si>
-  <si>
-    <t>Docente Participante</t>
-  </si>
-  <si>
-    <t>Actividades</t>
   </si>
   <si>
     <t>Departamento</t>
@@ -67,12 +50,36 @@
   <si>
     <t>Estado del Proyecto</t>
   </si>
+  <si>
+    <t>REGISTRO DE ESTUDIANTES DE PRÁCTICAS PROPROFESIONALES DE SERVICIO COMUNITARIO</t>
+  </si>
+  <si>
+    <t>Nombre del Proyecto Social</t>
+  </si>
+  <si>
+    <t>Código del Proyecto Social</t>
+  </si>
+  <si>
+    <t>Director de Proyecto</t>
+  </si>
+  <si>
+    <t>Docente Colaborador</t>
+  </si>
+  <si>
+    <t>Periodo del Proyecto</t>
+  </si>
+  <si>
+    <t>NRC</t>
+  </si>
+  <si>
+    <t>Descripcion del Proyecto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,13 +99,40 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -125,49 +159,50 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -185,133 +220,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2385060</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12374</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1" descr="Imagen de consulta de la búsqueda visual">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9DC82C9-45B8-9094-6C4C-39E0D45CB500}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="205740" y="449580"/>
-          <a:ext cx="2971800" cy="766754"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1375676</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>103318</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>418745</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2" descr="Computación Gráfica – Archivos Espe">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E508E97-75FD-C968-BB16-BFF5E73BB25F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="34655583" y="395713"/>
-          <a:ext cx="3420139" cy="865130"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -611,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE16FFB-0DBF-4542-BF2E-0694577CABAA}">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:V328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,123 +535,1070 @@
     <col min="7" max="7" width="30.6640625" customWidth="1"/>
     <col min="8" max="8" width="26.77734375" customWidth="1"/>
     <col min="9" max="9" width="41.109375" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" customWidth="1"/>
-    <col min="11" max="11" width="16.21875" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="10" max="10" width="30.77734375" customWidth="1"/>
+    <col min="11" max="11" width="31.33203125" customWidth="1"/>
+    <col min="12" max="12" width="25.77734375" customWidth="1"/>
     <col min="13" max="13" width="38.33203125" customWidth="1"/>
     <col min="14" max="14" width="25.44140625" customWidth="1"/>
     <col min="22" max="22" width="28.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="E1" s="3" t="s">
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="8" spans="1:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="8" spans="1:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
+      <c r="H8" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="I8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="K8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="9"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D38" s="9"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D41" s="9"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D43" s="9"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D44" s="9"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D45" s="9"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="9"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" s="9"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="9"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D52" s="9"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D53" s="9"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D54" s="9"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D55" s="9"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D56" s="9"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D57" s="9"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D59" s="9"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="9"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="9"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D62" s="9"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D63" s="9"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D64" s="9"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" s="9"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D66" s="9"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="9"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="9"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D69" s="9"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D70" s="9"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D71" s="9"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D72" s="9"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D73" s="9"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D74" s="9"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D75" s="9"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D76" s="9"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D77" s="9"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D78" s="9"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D79" s="9"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D80" s="9"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D81" s="9"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D82" s="9"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D83" s="9"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D84" s="9"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D85" s="9"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D86" s="9"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D87" s="9"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D88" s="9"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D89" s="9"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D90" s="9"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D91" s="9"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D92" s="9"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D93" s="9"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D94" s="9"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D95" s="9"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D96" s="9"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97" s="9"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D98" s="9"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D99" s="9"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D100" s="9"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D101" s="9"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D102" s="9"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D103" s="9"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D104" s="9"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D105" s="9"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D106" s="9"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D107" s="9"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D108" s="9"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D109" s="9"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D110" s="9"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D111" s="9"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D112" s="9"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D113" s="9"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D114" s="9"/>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D115" s="9"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D116" s="9"/>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D117" s="9"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D118" s="9"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D119" s="9"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D120" s="9"/>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D121" s="9"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D122" s="9"/>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D123" s="9"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D124" s="9"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D125" s="9"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D126" s="9"/>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D127" s="9"/>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D128" s="9"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D129" s="9"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D130" s="9"/>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D131" s="9"/>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D132" s="9"/>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D133" s="9"/>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D134" s="9"/>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D135" s="9"/>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D136" s="9"/>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D137" s="9"/>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D138" s="9"/>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D139" s="9"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D140" s="9"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D141" s="9"/>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D142" s="9"/>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D143" s="9"/>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D144" s="9"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D145" s="9"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D146" s="9"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D147" s="9"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D148" s="9"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D149" s="9"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D150" s="9"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D151" s="9"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D152" s="9"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D153" s="9"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D154" s="9"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D155" s="9"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D156" s="9"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D157" s="9"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D158" s="9"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D159" s="9"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D160" s="9"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D161" s="9"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D162" s="9"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D163" s="9"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D164" s="9"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D165" s="9"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D166" s="9"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D167" s="9"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D168" s="9"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D169" s="9"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D170" s="9"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D171" s="9"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D172" s="9"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D173" s="9"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D174" s="9"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D175" s="9"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D176" s="9"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D177" s="9"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D178" s="9"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D179" s="9"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D180" s="9"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D181" s="9"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D182" s="9"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D183" s="9"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D184" s="9"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D185" s="9"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D186" s="9"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D187" s="9"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D188" s="9"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D189" s="9"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D190" s="9"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D191" s="9"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D192" s="9"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D193" s="9"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D194" s="9"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D195" s="9"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D196" s="9"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D197" s="9"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D198" s="9"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D199" s="9"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D200" s="9"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D201" s="9"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D202" s="9"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D203" s="9"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D204" s="9"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D205" s="9"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D206" s="9"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D207" s="9"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D208" s="9"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D209" s="9"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D210" s="9"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D211" s="9"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D212" s="9"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D213" s="9"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D214" s="9"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D215" s="9"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D216" s="9"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D217" s="9"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D218" s="9"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D219" s="9"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D220" s="9"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D221" s="9"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D222" s="9"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D223" s="9"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D224" s="9"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D225" s="9"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D226" s="9"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D227" s="9"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D228" s="9"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D229" s="9"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D230" s="9"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D231" s="9"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D232" s="9"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D233" s="9"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D234" s="9"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D235" s="9"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D236" s="9"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D237" s="9"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D238" s="9"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D239" s="9"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D240" s="9"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D241" s="9"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D242" s="9"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D243" s="9"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D244" s="9"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D245" s="9"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D246" s="9"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D247" s="9"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D248" s="9"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D249" s="9"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D250" s="9"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D251" s="9"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D252" s="9"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D253" s="9"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D254" s="9"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D255" s="9"/>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D256" s="9"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D257" s="9"/>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D258" s="9"/>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D259" s="9"/>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D260" s="9"/>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D261" s="9"/>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D262" s="9"/>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D263" s="9"/>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D264" s="9"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D265" s="9"/>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D266" s="9"/>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D267" s="9"/>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D268" s="9"/>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D269" s="9"/>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D270" s="9"/>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D271" s="9"/>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D272" s="9"/>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D273" s="9"/>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D274" s="9"/>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D275" s="9"/>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D276" s="9"/>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D277" s="9"/>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D278" s="9"/>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D279" s="9"/>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D280" s="9"/>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D281" s="9"/>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D282" s="9"/>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D283" s="9"/>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D284" s="9"/>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D285" s="9"/>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D286" s="9"/>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D287" s="9"/>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D288" s="9"/>
+    </row>
+    <row r="289" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D289" s="9"/>
+    </row>
+    <row r="290" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D290" s="9"/>
+    </row>
+    <row r="291" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D291" s="9"/>
+    </row>
+    <row r="292" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D292" s="9"/>
+    </row>
+    <row r="293" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D293" s="9"/>
+    </row>
+    <row r="294" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D294" s="9"/>
+    </row>
+    <row r="295" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D295" s="9"/>
+    </row>
+    <row r="296" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D296" s="9"/>
+    </row>
+    <row r="297" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D297" s="9"/>
+    </row>
+    <row r="298" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D298" s="9"/>
+    </row>
+    <row r="299" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D299" s="9"/>
+    </row>
+    <row r="300" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D300" s="9"/>
+    </row>
+    <row r="301" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D301" s="9"/>
+    </row>
+    <row r="302" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D302" s="9"/>
+    </row>
+    <row r="303" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D303" s="9"/>
+    </row>
+    <row r="304" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D304" s="9"/>
+    </row>
+    <row r="305" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D305" s="9"/>
+    </row>
+    <row r="306" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D306" s="9"/>
+    </row>
+    <row r="307" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D307" s="9"/>
+    </row>
+    <row r="308" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D308" s="9"/>
+    </row>
+    <row r="309" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D309" s="9"/>
+    </row>
+    <row r="310" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D310" s="9"/>
+    </row>
+    <row r="311" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D311" s="9"/>
+    </row>
+    <row r="312" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D312" s="9"/>
+    </row>
+    <row r="313" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D313" s="9"/>
+    </row>
+    <row r="314" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D314" s="9"/>
+    </row>
+    <row r="315" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D315" s="9"/>
+    </row>
+    <row r="316" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D316" s="9"/>
+    </row>
+    <row r="317" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D317" s="9"/>
+    </row>
+    <row r="318" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D318" s="9"/>
+    </row>
+    <row r="319" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D319" s="9"/>
+    </row>
+    <row r="320" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D320" s="9"/>
+    </row>
+    <row r="321" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D321" s="9"/>
+    </row>
+    <row r="322" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D322" s="9"/>
+    </row>
+    <row r="323" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D323" s="9"/>
+    </row>
+    <row r="324" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D324" s="9"/>
+    </row>
+    <row r="325" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D325" s="9"/>
+    </row>
+    <row r="326" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D326" s="9"/>
+    </row>
+    <row r="327" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D327" s="9"/>
+    </row>
+    <row r="328" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D328" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E1:N1"/>
     <mergeCell ref="N9:V9"/>
     <mergeCell ref="N8:V8"/>
+    <mergeCell ref="B2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="33c8bdda-defa-435a-b09b-17c633094ed5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E3D40D7370BE704D9F987D37C7518305" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="713a4ab37a2269b86b211ad079bba34f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="33c8bdda-defa-435a-b09b-17c633094ed5" xmlns:ns4="5e78a4f3-a9b1-4fe1-9da0-d43cac8a1c9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="799d028bd5d959863f471fdad4996989" ns3:_="" ns4:_="">
     <xsd:import namespace="33c8bdda-defa-435a-b09b-17c633094ed5"/>
@@ -970,32 +1825,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80F8F01B-42E4-4ED9-9137-CD8DE7B67D7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5e78a4f3-a9b1-4fe1-9da0-d43cac8a1c9f"/>
-    <ds:schemaRef ds:uri="33c8bdda-defa-435a-b09b-17c633094ed5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F7F9947-D4DB-49D0-81FC-207E2ECAB2E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="33c8bdda-defa-435a-b09b-17c633094ed5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB6CAFB9-21A0-4331-A882-841105351FBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1012,4 +1859,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F7F9947-D4DB-49D0-81FC-207E2ECAB2E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80F8F01B-42E4-4ED9-9137-CD8DE7B67D7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5e78a4f3-a9b1-4fe1-9da0-d43cac8a1c9f"/>
+    <ds:schemaRef ds:uri="33c8bdda-defa-435a-b09b-17c633094ed5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>